<commit_message>
MOD: corrige errores y añade video sustentación
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP5"/>
+  <dimension ref="A1:AP17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -647,27 +647,27 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1101</v>
+        <v>1702</v>
       </c>
       <c r="B2" t="n">
-        <v>1101</v>
+        <v>1701</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD NACIONAL DE COLOMBIA</t>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Principal</t>
+          <t>Seccional</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>OFICIAL</t>
+          <t>PRIVADA</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -679,27 +679,27 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Bogotá D.C.</t>
+          <t>Valle Del Cauca</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>11001</v>
+        <v>76001</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Bogotá, D.C.</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>1042</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>INGENIERIA AGRONOMICA</t>
+          <t>INGENIERIA DE SISTEMAS Y COMPUTACION</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -712,17 +712,17 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>6</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Universitaria</t>
+          <t>Universitario</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -742,56 +742,62 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>824</t>
+          <t>827</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>Ingeniería agronómica, pecuaria y afines</t>
-        </is>
-      </c>
-      <c r="Y2" t="n">
-        <v>8</v>
+          <t>Ingeniería de sistemas, telemática y afines</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Agropecuario, Silvicultura, Pesca y Veterinaria</t>
-        </is>
-      </c>
-      <c r="AA2" t="n">
-        <v>81</v>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>Agropecuario</t>
-        </is>
-      </c>
-      <c r="AC2" t="n">
-        <v>811</v>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>Producción agrícola y ganadera</t>
+          <t>Uso de computadores</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>76</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>Bogotá D.C.</t>
+          <t>Valle Del Cauca</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>11001</t>
+          <t>76001</t>
         </is>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>Bogotá, D.C.</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="AI2" t="n">
@@ -809,41 +815,41 @@
         <v>1</v>
       </c>
       <c r="AM2" t="n">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="AN2" t="n">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="AO2" t="n">
-        <v>465</v>
+        <v>160</v>
       </c>
       <c r="AP2" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1101</v>
+        <v>1702</v>
       </c>
       <c r="B3" t="n">
-        <v>1101</v>
+        <v>1701</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD NACIONAL DE COLOMBIA</t>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Principal</t>
+          <t>Seccional</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>OFICIAL</t>
+          <t>PRIVADA</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -855,27 +861,27 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Bogotá D.C.</t>
+          <t>Valle Del Cauca</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>11001</v>
+        <v>76001</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Bogotá, D.C.</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>1042</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>INGENIERIA AGRONOMICA</t>
+          <t>INGENIERIA DE SISTEMAS Y COMPUTACION</t>
         </is>
       </c>
       <c r="O3" t="n">
@@ -888,17 +894,17 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>6</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Universitaria</t>
+          <t>Universitario</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -918,56 +924,62 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>824</t>
+          <t>827</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>Ingeniería agronómica, pecuaria y afines</t>
-        </is>
-      </c>
-      <c r="Y3" t="n">
-        <v>8</v>
+          <t>Ingeniería de sistemas, telemática y afines</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Agropecuario, Silvicultura, Pesca y Veterinaria</t>
-        </is>
-      </c>
-      <c r="AA3" t="n">
-        <v>81</v>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>Agropecuario</t>
-        </is>
-      </c>
-      <c r="AC3" t="n">
-        <v>811</v>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>Producción agrícola y ganadera</t>
+          <t>Uso de computadores</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>76</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>Bogotá D.C.</t>
+          <t>Valle Del Cauca</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>11001</t>
+          <t>76001</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>Bogotá, D.C.</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="AI3" t="n">
@@ -985,41 +997,41 @@
         <v>2</v>
       </c>
       <c r="AM3" t="n">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="AN3" t="n">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="AO3" t="n">
-        <v>466</v>
+        <v>163</v>
       </c>
       <c r="AP3" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1101</v>
+        <v>1702</v>
       </c>
       <c r="B4" t="n">
-        <v>1101</v>
+        <v>1701</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD NACIONAL DE COLOMBIA</t>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Principal</t>
+          <t>Seccional</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>OFICIAL</t>
+          <t>PRIVADA</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -1031,27 +1043,27 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Bogotá D.C.</t>
+          <t>Valle Del Cauca</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>11001</v>
+        <v>76001</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Bogotá, D.C.</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>1042</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>INGENIERIA AGRONOMICA</t>
+          <t>INGENIERIA DE SISTEMAS Y COMPUTACION</t>
         </is>
       </c>
       <c r="O4" t="n">
@@ -1064,17 +1076,17 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>6</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Universitaria</t>
+          <t>Universitario</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -1094,56 +1106,62 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>824</t>
+          <t>827</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>Ingeniería agronómica, pecuaria y afines</t>
-        </is>
-      </c>
-      <c r="Y4" t="n">
-        <v>8</v>
+          <t>Ingeniería de sistemas, telemática y afines</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>Agropecuario, Silvicultura, Pesca y Veterinaria</t>
-        </is>
-      </c>
-      <c r="AA4" t="n">
-        <v>81</v>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Agropecuario</t>
-        </is>
-      </c>
-      <c r="AC4" t="n">
-        <v>811</v>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>Producción agrícola y ganadera</t>
+          <t>Uso de computadores</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>76</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>Bogotá D.C.</t>
+          <t>Valle Del Cauca</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>11001</t>
+          <t>76001</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>Bogotá, D.C.</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="AI4" t="n">
@@ -1161,41 +1179,39 @@
         <v>1</v>
       </c>
       <c r="AM4" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="AN4" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AO4" t="n">
-        <v>253</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="AP4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1101</v>
+        <v>1702</v>
       </c>
       <c r="B5" t="n">
-        <v>1101</v>
+        <v>1701</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>UNIVERSIDAD NACIONAL DE COLOMBIA</t>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Principal</t>
+          <t>Seccional</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>OFICIAL</t>
+          <t>PRIVADA</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -1207,27 +1223,27 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Bogotá D.C.</t>
+          <t>Valle Del Cauca</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>11001</v>
+        <v>76001</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Bogotá, D.C.</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>1042</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>INGENIERIA AGRONOMICA</t>
+          <t>INGENIERIA DE SISTEMAS Y COMPUTACION</t>
         </is>
       </c>
       <c r="O5" t="n">
@@ -1240,17 +1256,17 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>6</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>Universitaria</t>
+          <t>Universitario</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -1270,56 +1286,62 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>824</t>
+          <t>827</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>Ingeniería agronómica, pecuaria y afines</t>
-        </is>
-      </c>
-      <c r="Y5" t="n">
-        <v>8</v>
+          <t>Ingeniería de sistemas, telemática y afines</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>Agropecuario, Silvicultura, Pesca y Veterinaria</t>
-        </is>
-      </c>
-      <c r="AA5" t="n">
-        <v>81</v>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>Agropecuario</t>
-        </is>
-      </c>
-      <c r="AC5" t="n">
-        <v>811</v>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>Producción agrícola y ganadera</t>
+          <t>Uso de computadores</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>76</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>Bogotá D.C.</t>
+          <t>Valle Del Cauca</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>11001</t>
+          <t>76001</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>Bogotá, D.C.</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="AI5" t="n">
@@ -1337,15 +1359,2195 @@
         <v>2</v>
       </c>
       <c r="AM5" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="AN5" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="AO5" t="n">
-        <v>276</v>
-      </c>
-      <c r="AP5" t="n">
+        <v>25</v>
+      </c>
+      <c r="AP5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>76</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>1042</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>INGENIERIA DE SISTEMAS Y COMPUTACION</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>827</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Ingeniería de sistemas, telemática y afines</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>Uso de computadores</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="AK6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>34</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>76</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>1042</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>INGENIERIA DE SISTEMAS Y COMPUTACION</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>827</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Ingeniería de sistemas, telemática y afines</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>Uso de computadores</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="AK7" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>28</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>178</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>76</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>1042</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>INGENIERIA DE SISTEMAS Y COMPUTACION</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>827</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Ingeniería de sistemas, telemática y afines</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>Uso de computadores</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="AK8" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>26</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>4</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>76</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>1042</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>INGENIERIA DE SISTEMAS Y COMPUTACION</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>827</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>Ingeniería de sistemas, telemática y afines</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>Tecnologías de la Información y la Comunicación (TIC)</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>Uso de computadores</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="AK9" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>24</v>
+      </c>
+      <c r="AP9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>76</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>1043</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>INGENIERIA ELECTRONICA</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>829</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>Ingeniería electrónica, telecomunicaciones y afines</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>Ingeniería, Industria y Construcción</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>Ingeniería y profesiones afines</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>714</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>Electrónica y automatización</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="AK10" t="n">
+        <v>2020</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>19</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>19</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>152</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>76</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>1043</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>INGENIERIA ELECTRONICA</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>829</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>Ingeniería electrónica, telecomunicaciones y afines</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>Ingeniería, Industria y Construcción</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>Ingeniería y profesiones afines</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>714</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>Electrónica y automatización</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="AK11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>6</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>6</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>140</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>76</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>1043</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>INGENIERIA ELECTRONICA</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>829</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>Ingeniería electrónica, telecomunicaciones y afines</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>Ingeniería, Industria y Construcción</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>Ingeniería y profesiones afines</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>714</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>Electrónica y automatización</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH12" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ12" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="AK12" t="n">
+        <v>2020</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>33</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>4</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>76</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>1043</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>INGENIERIA ELECTRONICA</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>829</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>Ingeniería electrónica, telecomunicaciones y afines</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>Ingeniería, Industria y Construcción</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>Ingeniería y profesiones afines</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>714</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>Electrónica y automatización</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="AK13" t="n">
+        <v>2020</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>30</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>76</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>1043</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>INGENIERIA ELECTRONICA</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>829</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>Ingeniería electrónica, telecomunicaciones y afines</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>Ingeniería, Industria y Construcción</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Ingeniería y profesiones afines</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>714</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>Electrónica y automatización</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ14" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="AK14" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>122</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>4</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>76</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>1043</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>INGENIERIA ELECTRONICA</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>829</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>Ingeniería electrónica, telecomunicaciones y afines</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>Ingeniería, Industria y Construcción</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>Ingeniería y profesiones afines</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>714</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>Electrónica y automatización</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="AK15" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>18</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>15</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>120</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>4</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>76</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>1043</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>INGENIERIA ELECTRONICA</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>829</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>Ingeniería electrónica, telecomunicaciones y afines</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>Ingeniería, Industria y Construcción</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>Ingeniería y profesiones afines</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>714</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>Electrónica y automatización</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="AK16" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>26</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1702</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1701</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>PONTIFICIA UNIVERSIDAD JAVERIANA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Seccional</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>PRIVADA</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>4</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>76</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>76001</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>1043</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>INGENIERIA ELECTRONICA</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>1</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>PREGRADO</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Universitario</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Presencial</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>Ingeniería, arquitectura, urbanismo y afines</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>829</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>Ingeniería electrónica, telecomunicaciones y afines</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>Ingeniería, Industria y Construcción</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Ingeniería y profesiones afines</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>714</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>Electrónica y automatización</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>Valle Del Cauca</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>76001</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="AI17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="AK17" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>26</v>
+      </c>
+      <c r="AP17" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>